<commit_message>
Make metadata same accross roles (#760)
* fix issue

* fix issue

* fixes

* add tests for cdm extension

* changelog updated

* redo metadata

* fix issues

* additional fixes

* removing support for loading classic cdf

* fix

* cleansing

* add missing aspect

* fix tests

* fix test

* skipping tests that are leveraging referenceØ

* changelog

* revert missing docstring

* update

* update gitignore
</commit_message>
<xml_diff>
--- a/cognite/neat/_rules/catalog/info-rules-imf.xlsx
+++ b/cognite/neat/_rules/catalog/info-rules-imf.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/cognite/neat/rules/catalog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/cognite/neat/_rules/catalog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8D2F11-87B9-5C42-B8F9-FA67686FBA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED9B58D-116A-CC45-87FC-4AC2E707C6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Classes" sheetId="4" r:id="rId2"/>
     <sheet name="Properties" sheetId="2" r:id="rId3"/>
+    <sheet name="Prefixes" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="tmp" localSheetId="2">Properties!$A$1:$J$1</definedName>
@@ -126,21 +127,6 @@
     <t>Match Type</t>
   </si>
   <si>
-    <t>namespace</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>license</t>
-  </si>
-  <si>
-    <t>rights</t>
-  </si>
-  <si>
     <t>Parent Class</t>
   </si>
   <si>
@@ -186,19 +172,10 @@
     <t>dataModelType</t>
   </si>
   <si>
-    <t>enterprise</t>
-  </si>
-  <si>
     <t>extension</t>
   </si>
   <si>
     <t>addition</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>complete</t>
   </si>
   <si>
     <t>imf</t>
@@ -214,12 +191,6 @@
   </si>
   <si>
     <t>Nikola Vasiljevic</t>
-  </si>
-  <si>
-    <t>CC BY 4.0</t>
-  </si>
-  <si>
-    <t>Free to use</t>
   </si>
   <si>
     <t>predicate</t>
@@ -313,6 +284,36 @@
   </si>
   <si>
     <t>imf:uom</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>external_id</t>
+  </si>
+  <si>
+    <t>imfTypes</t>
+  </si>
+  <si>
+    <t>imfSpace</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>Namespace</t>
+  </si>
+  <si>
+    <t>partial</t>
+  </si>
+  <si>
+    <t>solution</t>
   </si>
 </sst>
 </file>
@@ -714,10 +715,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:S1000"/>
+  <dimension ref="A1:S998"/>
   <sheetViews>
-    <sheetView zoomScale="296" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="296" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -735,16 +736,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C1"/>
     </row>
     <row r="2" spans="1:19" ht="16">
       <c r="A2" s="14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
-      <c r="B2" t="s">
-        <v>42</v>
+      <c r="B2" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="C2"/>
     </row>
@@ -753,7 +754,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -770,10 +771,10 @@
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -790,10 +791,10 @@
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -810,10 +811,10 @@
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1">
       <c r="A6" s="14" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>48</v>
+      <c r="B6" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -830,10 +831,10 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1">
       <c r="A7" s="14" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -853,7 +854,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -872,8 +873,8 @@
       <c r="A9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>45</v>
+      <c r="B9" s="16" t="s">
+        <v>77</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -933,7 +934,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -951,12 +952,7 @@
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>52</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="C13" s="11"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -976,12 +972,7 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>53</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="C14" s="11"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -5081,44 +5072,10 @@
       <c r="S218" s="1"/>
     </row>
     <row r="219" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A219" s="1"/>
-      <c r="C219" s="11"/>
-      <c r="D219" s="1"/>
-      <c r="E219" s="1"/>
-      <c r="F219" s="1"/>
-      <c r="G219" s="1"/>
-      <c r="H219" s="1"/>
-      <c r="I219" s="1"/>
-      <c r="J219" s="1"/>
-      <c r="K219" s="1"/>
-      <c r="L219" s="1"/>
-      <c r="M219" s="1"/>
-      <c r="N219" s="1"/>
-      <c r="O219" s="1"/>
-      <c r="P219" s="1"/>
-      <c r="Q219" s="1"/>
-      <c r="R219" s="1"/>
-      <c r="S219" s="1"/>
+      <c r="C219" s="12"/>
     </row>
     <row r="220" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A220" s="1"/>
-      <c r="C220" s="11"/>
-      <c r="D220" s="1"/>
-      <c r="E220" s="1"/>
-      <c r="F220" s="1"/>
-      <c r="G220" s="1"/>
-      <c r="H220" s="1"/>
-      <c r="I220" s="1"/>
-      <c r="J220" s="1"/>
-      <c r="K220" s="1"/>
-      <c r="L220" s="1"/>
-      <c r="M220" s="1"/>
-      <c r="N220" s="1"/>
-      <c r="O220" s="1"/>
-      <c r="P220" s="1"/>
-      <c r="Q220" s="1"/>
-      <c r="R220" s="1"/>
-      <c r="S220" s="1"/>
+      <c r="C220" s="12"/>
     </row>
     <row r="221" spans="1:19" ht="15.75" customHeight="1">
       <c r="C221" s="12"/>
@@ -7454,16 +7411,7 @@
     <row r="998" spans="3:3" ht="15.75" customHeight="1">
       <c r="C998" s="12"/>
     </row>
-    <row r="999" spans="3:3" ht="15.75" customHeight="1">
-      <c r="C999" s="12"/>
-    </row>
-    <row r="1000" spans="3:3" ht="15.75" customHeight="1">
-      <c r="C1000" s="12"/>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{57F68BEB-B928-854D-8D34-20C38200CBBB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -7477,7 +7425,7 @@
   <dimension ref="A1:X993"/>
   <sheetViews>
     <sheetView zoomScale="134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -7491,19 +7439,19 @@
   <sheetData>
     <row r="1" spans="1:24" ht="32">
       <c r="A1" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>19</v>
@@ -7538,7 +7486,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>12</v>
@@ -7550,14 +7498,14 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C3" s="18"/>
       <c r="E3" s="18" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -8561,7 +8509,7 @@
   </sheetPr>
   <dimension ref="A1:Q928"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -8595,25 +8543,25 @@
         <v>17</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17.25" customHeight="1">
@@ -8633,16 +8581,16 @@
         <v>6</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>12</v>
@@ -8659,14 +8607,14 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C3" s="9"/>
       <c r="E3" s="10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
@@ -8676,25 +8624,25 @@
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C4" s="9"/>
       <c r="E4" s="10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F4" s="10">
         <v>0</v>
@@ -8704,25 +8652,25 @@
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C5" s="9"/>
       <c r="E5" s="10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -8732,25 +8680,25 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="19" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C6" s="9"/>
       <c r="E6" s="10" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F6" s="10">
         <v>0</v>
@@ -8760,25 +8708,25 @@
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C7" s="9"/>
       <c r="E7" s="10" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F7" s="10">
         <v>0</v>
@@ -8788,81 +8736,81 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="19" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C8" s="9"/>
       <c r="E8" s="19" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F8" s="10">
         <v>0</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="19" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C9" s="9"/>
       <c r="E9" s="19" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F9" s="10">
         <v>0</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="19" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C10" s="9"/>
       <c r="E10" s="19" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F10" s="10">
         <v>0</v>
@@ -8872,13 +8820,13 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="19" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1">
@@ -17147,4 +17095,38 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8173E552-7960-7C45-9594-F37EF2AA195E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{EC305E71-C927-7A40-B465-2EF3AEB8A6E0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>